<commit_message>
Added notifications and wathlist module test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="5250"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCase_A7" sheetId="2" r:id="rId2"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId3"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1:D16"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -33,24 +33,6 @@
     <t>Results</t>
   </si>
   <si>
-    <t>USERNAME</t>
-  </si>
-  <si>
-    <t>PASSWORD</t>
-  </si>
-  <si>
-    <t>ACCOUNT NAME</t>
-  </si>
-  <si>
-    <t>VALIDITY</t>
-  </si>
-  <si>
-    <t>YES</t>
-  </si>
-  <si>
-    <t>NO</t>
-  </si>
-  <si>
     <t>TestCase_A1</t>
   </si>
   <si>
@@ -63,55 +45,28 @@
     <t>TC STEPS</t>
   </si>
   <si>
-    <t>amneetsingh72@gmail.com</t>
-  </si>
-  <si>
-    <t>amneetsingh100@gmail.com</t>
-  </si>
-  <si>
-    <t>amneet singh</t>
-  </si>
-  <si>
-    <t>random</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>To verify that Linkedin login is working correctly</t>
-  </si>
-  <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>transaction@2</t>
-  </si>
-  <si>
-    <t>TestCase_A7</t>
-  </si>
-  <si>
     <t>TestCase_A3</t>
   </si>
   <si>
     <t>TestCase_A4</t>
   </si>
   <si>
-    <t>N</t>
+    <t>To verify that new user is able to register TR new account and login with that</t>
+  </si>
+  <si>
+    <t>To verify that existing TR user is able to login successfully</t>
+  </si>
+  <si>
+    <t>To verify that existing LI user credentials are working fine</t>
+  </si>
+  <si>
+    <t>To verify that existing FB user credentials are working fine</t>
   </si>
   <si>
     <t>SKIP</t>
-  </si>
-  <si>
-    <t>To verify that new user is able to register TR new account and login with that</t>
-  </si>
-  <si>
-    <t>To verify that existing TR user is able to login successfully</t>
-  </si>
-  <si>
-    <t>To verify that existing LI user credentials are working fine</t>
-  </si>
-  <si>
-    <t>To verify that existing FB user credentials are working fine</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -122,20 +77,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -184,30 +132,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="top"/>
-      <protection locked="0"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -535,74 +477,61 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2" t="s">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>29</v>
+        <v>13</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>27</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -610,119 +539,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="35.28515625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.85546875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="11.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" ht="13.5" customHeight="1">
-      <c r="A2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
-      <c r="A3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2" display="welcome@12"/>
-    <hyperlink ref="A4" r:id="rId3" display="amneetsinghasr@gmail.com"/>
-    <hyperlink ref="A3" r:id="rId4"/>
-    <hyperlink ref="B2" r:id="rId5"/>
-    <hyperlink ref="B3" r:id="rId6"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -730,37 +547,37 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="4" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="4" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="4" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="4" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>14</v>
+      <c r="B1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
     </row>
     <row r="3" spans="1:3" ht="196.5" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
-      <c r="C3" s="6"/>
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
     </row>
     <row r="4" spans="1:3" ht="252.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Running all the suites by making runmode as Y in the excel sheets
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -11,11 +11,12 @@
     <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t>TCID</t>
   </si>
@@ -63,22 +64,12 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -457,10 +448,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -488,7 +479,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -499,7 +490,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -513,7 +504,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -527,7 +518,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -540,7 +531,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
@@ -548,10 +539,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Changes in the following files: 1)AuthoringDeleteTest.java 2)AuthoringProfileCommentsTest.java 3)Changing the runmodes in excels to run only these 2 TCs
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -64,12 +64,19 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -448,10 +455,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -479,7 +486,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -490,7 +497,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -504,7 +511,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -518,7 +525,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -539,10 +546,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Running only Suite A
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
   <si>
     <t>TCID</t>
   </si>
@@ -64,12 +64,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -79,7 +73,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -458,10 +451,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="70.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -489,7 +482,7 @@
         <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -500,7 +493,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>14</v>
@@ -514,7 +507,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>14</v>
@@ -528,7 +521,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>14</v>
@@ -549,10 +542,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Added 2 new test cases: TestCase_A5 TestCase_A6
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -8,15 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId2"/>
+    <sheet name="TestCase_A5" sheetId="5" r:id="rId2"/>
+    <sheet name="TestCase_A6" sheetId="6" r:id="rId3"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="125725"/>
-  <oleSize ref="A1"/>
+  <oleSize ref="A1:D11"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -63,16 +65,37 @@
     <t>Y</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SKIP</t>
+  </si>
+  <si>
+    <t>TestCase_A5</t>
+  </si>
+  <si>
+    <t>To verify FIRST NAME field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>VALIDITY</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>CHARACTER LENGTH</t>
   </si>
   <si>
     <t>PASS</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>SKIP</t>
+    <t>TestCase_A6</t>
+  </si>
+  <si>
+    <t>To verify LAST NAME field in new TR user registration page</t>
   </si>
 </sst>
 </file>
@@ -80,7 +103,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -95,6 +118,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -135,10 +165,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="top"/>
+      <protection locked="0"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -151,8 +185,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -450,7 +487,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
@@ -486,10 +523,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -500,10 +537,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -514,10 +551,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -528,10 +565,38 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="B6" s="6" t="s">
         <v>18</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -541,10 +606,170 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7">
+        <v>69</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7">
+        <v>70</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7">
+        <v>71</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Changes in TestCase_A6.java and A suite.xlsx
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="13290" windowHeight="3900" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -487,7 +487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -686,8 +686,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -718,7 +718,7 @@
         <v>20</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
@@ -732,7 +732,7 @@
         <v>20</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>23</v>

</xml_diff>

<commit_message>
Running whole suite A
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
   <si>
     <t>TCID</t>
   </si>
@@ -95,9 +95,6 @@
   </si>
   <si>
     <t>To verify LAST NAME field in new TR user registration page</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N </t>
   </si>
 </sst>
 </file>
@@ -491,7 +488,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -538,7 +535,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>16</v>
@@ -552,7 +549,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>16</v>
@@ -566,7 +563,7 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Running entire suite a
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>SKIP</t>
@@ -488,7 +485,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,7 +521,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -535,10 +532,10 @@
         <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -549,10 +546,10 @@
         <v>12</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -563,38 +560,38 @@
         <v>13</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>15</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +604,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,16 +615,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -635,13 +632,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -649,13 +646,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -663,13 +660,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +695,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -715,13 +712,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -729,13 +726,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -743,13 +740,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
New Script Implementation done and code changes done authoring functionality New Script Implementation 1.AuthoirngRecordViewDetailsTest.java 2.AppHeaderFooterLinkValidationTest.java 3.ApplicationLinksValidationTest.java
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="25">
   <si>
     <t>TCID</t>
   </si>
@@ -62,9 +62,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>SKIP</t>
@@ -488,7 +485,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -524,7 +521,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -538,7 +535,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -552,7 +549,7 @@
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -566,35 +563,35 @@
         <v>14</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>18</v>
-      </c>
       <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="C7" s="6" t="s">
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -607,7 +604,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -618,16 +615,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -635,13 +632,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -649,13 +646,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -663,13 +660,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -698,10 +695,10 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -715,13 +712,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -729,13 +726,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -743,13 +740,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running all the test cases in Chrome
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -10,14 +10,17 @@
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
     <sheet name="TestCase_A5" sheetId="5" r:id="rId2"/>
     <sheet name="TestCase_A6" sheetId="6" r:id="rId3"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId4"/>
+    <sheet name="TestCase_A7" sheetId="7" r:id="rId4"/>
+    <sheet name="TestCase_A8" sheetId="8" r:id="rId5"/>
+    <sheet name="TestCase_A9" sheetId="9" r:id="rId6"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId7"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="41">
   <si>
     <t>TCID</t>
   </si>
@@ -94,14 +97,58 @@
     <t>To verify LAST NAME field in new TR user registration page</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>TestCase_A7</t>
+  </si>
+  <si>
+    <t>To verify that user is not able to login using FB option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>amneetsingh50@gmail.com</t>
+  </si>
+  <si>
+    <t>Transaction@2</t>
+  </si>
+  <si>
+    <t>amneetsingh500@gmail.com</t>
+  </si>
+  <si>
+    <t>transaction@2</t>
+  </si>
+  <si>
+    <t>EMAIL</t>
+  </si>
+  <si>
+    <t>TestCase_A8</t>
+  </si>
+  <si>
+    <t>To verify that user is not able to login using LI option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>amneetsingh100@gmail.com</t>
+  </si>
+  <si>
+    <t>amneetsingh10@gmail.com</t>
+  </si>
+  <si>
+    <t>TestCase_A9</t>
+  </si>
+  <si>
+    <t>To verify that user is not able to login using TR option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>amneet.singh@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>amneetsingh@thomsonreuters.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -486,18 +533,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="70.140625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="103.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -581,7 +628,7 @@
         <v>14</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -595,7 +642,49 @@
         <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -608,13 +697,13 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -628,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -642,7 +731,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -656,7 +745,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -693,8 +782,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -708,7 +797,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -722,7 +811,7 @@
         <v>14</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -736,7 +825,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -765,6 +854,366 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2"/>
+      <c r="B7" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4"/>
+    <hyperlink ref="A4" r:id="rId5"/>
+    <hyperlink ref="B4" r:id="rId6"/>
+    <hyperlink ref="A6" r:id="rId7"/>
+    <hyperlink ref="B7" r:id="rId8"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
@@ -773,10 +1222,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
Adding IAM test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -13,14 +13,17 @@
     <sheet name="TestCase_A7" sheetId="7" r:id="rId4"/>
     <sheet name="TestCase_A8" sheetId="8" r:id="rId5"/>
     <sheet name="TestCase_A9" sheetId="9" r:id="rId6"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId7"/>
+    <sheet name="TestCase_A10" sheetId="10" r:id="rId7"/>
+    <sheet name="TestCase_A11" sheetId="11" r:id="rId8"/>
+    <sheet name="TestCase_A12" sheetId="12" r:id="rId9"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -55,15 +58,6 @@
     <t>To verify that new user is able to register TR new account and login with that</t>
   </si>
   <si>
-    <t>To verify that existing TR user is able to login successfully</t>
-  </si>
-  <si>
-    <t>To verify that existing LI user credentials are working fine</t>
-  </si>
-  <si>
-    <t>To verify that existing FB user credentials are working fine</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -143,12 +137,97 @@
   </si>
   <si>
     <t>amneetsingh@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>To verify EMAIL ADDRESS field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>TestCase_A10</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SUFFIX</t>
+  </si>
+  <si>
+    <t>@abc.com</t>
+  </si>
+  <si>
+    <t>ERROR TEXT</t>
+  </si>
+  <si>
+    <t>Please enter no more than 70 characters.</t>
+  </si>
+  <si>
+    <t>Please enter a valid Email Address.</t>
+  </si>
+  <si>
+    <t>TestCase_A11</t>
+  </si>
+  <si>
+    <t>To verify CONFIRM PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>TestCase_A12</t>
+  </si>
+  <si>
+    <t>To verify PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>STRENGTH</t>
+  </si>
+  <si>
+    <t>TICK MARKS</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>Tr</t>
+  </si>
+  <si>
+    <t>Tra</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Transact</t>
+  </si>
+  <si>
+    <t>Transact2</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TestCase_A13</t>
+  </si>
+  <si>
+    <t>To verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
+  </si>
+  <si>
+    <t>To verify that existing TR user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>To verify that existing FB user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>To verify that existing LI user is able to login and logout successfully</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -218,7 +297,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -233,6 +312,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -240,11 +320,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -533,18 +608,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="103.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="103.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -569,10 +644,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -580,13 +655,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -594,13 +669,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -608,84 +683,187 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>40</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C11" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="196.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="252.75" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -697,27 +875,27 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -725,13 +903,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -739,13 +917,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -753,13 +931,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -777,27 +955,27 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -805,13 +983,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -819,13 +997,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -833,13 +1011,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -857,104 +1035,104 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -977,104 +1155,104 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1097,104 +1275,104 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1214,45 +1392,347 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="196.5" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="252.75" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="Transaction@2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4" display="transaction@2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new script implementation for authroing scripts, 1.Prevent bot functionality for same article 2.Prevent bot functionality for different article
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -13,14 +13,17 @@
     <sheet name="TestCase_A7" sheetId="7" r:id="rId4"/>
     <sheet name="TestCase_A8" sheetId="8" r:id="rId5"/>
     <sheet name="TestCase_A9" sheetId="9" r:id="rId6"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId7"/>
+    <sheet name="TestCase_A10" sheetId="10" r:id="rId7"/>
+    <sheet name="TestCase_A11" sheetId="11" r:id="rId8"/>
+    <sheet name="TestCase_A12" sheetId="12" r:id="rId9"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId10"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
   <si>
     <t>TCID</t>
   </si>
@@ -55,15 +58,6 @@
     <t>To verify that new user is able to register TR new account and login with that</t>
   </si>
   <si>
-    <t>To verify that existing TR user is able to login successfully</t>
-  </si>
-  <si>
-    <t>To verify that existing LI user credentials are working fine</t>
-  </si>
-  <si>
-    <t>To verify that existing FB user credentials are working fine</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -143,6 +137,90 @@
   </si>
   <si>
     <t>amneetsingh@thomsonreuters.com</t>
+  </si>
+  <si>
+    <t>To verify EMAIL ADDRESS field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>TestCase_A10</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>SUFFIX</t>
+  </si>
+  <si>
+    <t>@abc.com</t>
+  </si>
+  <si>
+    <t>ERROR TEXT</t>
+  </si>
+  <si>
+    <t>Please enter no more than 70 characters.</t>
+  </si>
+  <si>
+    <t>Please enter a valid Email Address.</t>
+  </si>
+  <si>
+    <t>TestCase_A11</t>
+  </si>
+  <si>
+    <t>To verify CONFIRM PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>TestCase_A12</t>
+  </si>
+  <si>
+    <t>To verify PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>STRENGTH</t>
+  </si>
+  <si>
+    <t>TICK MARKS</t>
+  </si>
+  <si>
+    <t>T</t>
+  </si>
+  <si>
+    <t>Weak</t>
+  </si>
+  <si>
+    <t>Tr</t>
+  </si>
+  <si>
+    <t>Tra</t>
+  </si>
+  <si>
+    <t>Good</t>
+  </si>
+  <si>
+    <t>Transact</t>
+  </si>
+  <si>
+    <t>Transact2</t>
+  </si>
+  <si>
+    <t>Strong</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>TestCase_A13</t>
+  </si>
+  <si>
+    <t>To verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
+  </si>
+  <si>
+    <t>To verify that existing TR user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>To verify that existing FB user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>To verify that existing LI user is able to login and logout successfully</t>
   </si>
 </sst>
 </file>
@@ -218,7 +296,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -233,6 +311,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -240,11 +319,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -533,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -569,10 +643,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -580,13 +654,13 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -594,13 +668,13 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>12</v>
+        <v>65</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -608,84 +682,187 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="6" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="6" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="6" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>14</v>
+        <v>23</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="6" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="6" t="s">
-        <v>14</v>
+        <v>31</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="6" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>22</v>
-      </c>
+      <c r="C11" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="48" customHeight="1">
+      <c r="A2" s="5"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+    </row>
+    <row r="3" spans="1:3" ht="196.5" customHeight="1">
+      <c r="A3" s="5"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="5"/>
+    </row>
+    <row r="4" spans="1:3" ht="252.75" customHeight="1">
+      <c r="A4" s="5"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -697,7 +874,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -708,16 +885,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -725,13 +902,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -739,13 +916,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -753,13 +930,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -777,7 +954,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -788,16 +965,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -805,13 +982,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -819,13 +996,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -833,13 +1010,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -857,7 +1034,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -869,92 +1046,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B4" s="7" t="s">
-        <v>31</v>
-      </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -977,7 +1154,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -989,92 +1166,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1097,7 +1274,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1109,92 +1286,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -1214,45 +1391,347 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="48" customHeight="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-    </row>
-    <row r="3" spans="1:3" ht="196.5" customHeight="1">
-      <c r="A3" s="5"/>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-    </row>
-    <row r="4" spans="1:3" ht="252.75" customHeight="1">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="7">
+        <v>61</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7">
+        <v>62</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7">
+        <v>63</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2">
+        <v>11</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="7"/>
+      <c r="D6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2" display="Transaction@2"/>
+    <hyperlink ref="A3" r:id="rId3"/>
+    <hyperlink ref="B3" r:id="rId4" display="transaction@2"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="2">
+        <v>2</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C5" s="2">
+        <v>4</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Commiting new test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="65">
   <si>
     <t>TCID</t>
   </si>
@@ -143,9 +143,6 @@
   </si>
   <si>
     <t>TestCase_A10</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
   <si>
     <t>SUFFIX</t>
@@ -610,7 +607,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -654,7 +651,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -668,7 +665,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -682,7 +679,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -777,10 +774,10 @@
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>46</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>47</v>
       </c>
       <c r="C12" s="2" t="s">
         <v>11</v>
@@ -791,10 +788,10 @@
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="B13" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>11</v>
@@ -805,10 +802,10 @@
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="5" t="s">
         <v>61</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>62</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>11</v>
@@ -894,7 +891,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -974,7 +971,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1055,7 +1052,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1175,7 +1172,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1274,7 +1271,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1295,7 +1292,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1394,7 +1391,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1410,10 +1407,10 @@
         <v>18</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1422,7 +1419,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1430,14 +1427,14 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>12</v>
@@ -1448,14 +1445,14 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -1466,16 +1463,16 @@
         <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>12</v>
@@ -1487,7 +1484,7 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>17</v>
@@ -1504,7 +1501,7 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
@@ -1533,7 +1530,7 @@
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:D1"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1554,7 +1551,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1601,7 +1598,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1618,10 +1615,10 @@
         <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>15</v>
@@ -1630,15 +1627,15 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1650,15 +1647,15 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -1667,7 +1664,7 @@
         <v>17</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
@@ -1675,10 +1672,10 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>55</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>56</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -1687,7 +1684,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>12</v>
@@ -1695,10 +1692,10 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -1707,7 +1704,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>12</v>
@@ -1715,10 +1712,10 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -1727,7 +1724,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
adding 2 more test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -218,6 +218,18 @@
   </si>
   <si>
     <t>To verify that existing LI user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>TestCase_A14</t>
+  </si>
+  <si>
+    <t>To verify that user is not able to submit new TR user registration form without filling in the required fields</t>
+  </si>
+  <si>
+    <t>TestCase_A15</t>
+  </si>
+  <si>
+    <t>To verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
   </si>
 </sst>
 </file>
@@ -604,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -813,6 +825,30 @@
       <c r="D14" s="2" t="s">
         <v>19</v>
       </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Running TestCase_A14 and TestCase_A15
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="70">
   <si>
     <t>TCID</t>
   </si>
@@ -230,6 +230,9 @@
   </si>
   <si>
     <t>To verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -619,7 +622,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,7 +655,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -666,7 +669,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -680,7 +683,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -694,7 +697,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -708,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -722,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -736,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -750,7 +753,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -764,7 +767,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -778,7 +781,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -792,7 +795,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -806,7 +809,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -820,7 +823,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>19</v>

</xml_diff>

<commit_message>
Running A1 and B1
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -622,7 +622,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C3" sqref="C3:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,7 +669,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -683,7 +683,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -697,7 +697,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -711,7 +711,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -725,7 +725,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -739,7 +739,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -753,7 +753,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -767,7 +767,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -781,7 +781,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -795,7 +795,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -809,7 +809,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -837,7 +837,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -851,7 +851,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>69</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Running suites a and b
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="69">
   <si>
     <t>TCID</t>
   </si>
@@ -230,9 +230,6 @@
   </si>
   <si>
     <t>To verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -622,7 +619,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -669,7 +666,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -683,7 +680,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -697,7 +694,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -711,7 +708,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -725,7 +722,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -739,7 +736,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -753,7 +750,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -767,7 +764,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -781,7 +778,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -795,7 +792,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -809,7 +806,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -823,7 +820,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -837,7 +834,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -851,7 +848,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Adding search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -892,10 +892,10 @@
         <v>72</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Watchlist test cases modified
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -251,6 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -639,10 +640,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -912,10 +913,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -959,8 +960,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1039,8 +1040,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1119,9 +1120,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1239,9 +1240,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1359,9 +1360,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1479,10 +1480,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1618,9 +1619,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1686,11 +1687,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Running suites A,B and E
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1348" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -242,16 +242,12 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -635,15 +631,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -668,7 +664,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -696,7 +692,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -710,7 +706,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -724,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -738,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -752,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -766,7 +762,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -780,7 +776,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -794,7 +790,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -808,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -822,7 +818,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -836,7 +832,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -850,7 +846,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -864,7 +860,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -878,7 +874,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -891,8 +887,8 @@
       <c r="B18" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>73</v>
+      <c r="C18" s="2" t="s">
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>
@@ -913,10 +909,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -960,8 +956,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1040,8 +1036,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1120,9 +1116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1240,9 +1236,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1360,9 +1356,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1480,10 +1476,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1619,9 +1615,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1687,11 +1683,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Taking latest code and Adding my changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -832,10 +835,10 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4">

</xml_diff>

<commit_message>
running D suite only
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -251,6 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -639,10 +640,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -838,7 +839,7 @@
         <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -912,10 +913,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -959,8 +960,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1039,8 +1040,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1119,9 +1120,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1239,9 +1240,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1359,9 +1360,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1479,10 +1480,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1618,9 +1619,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1686,11 +1687,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Taking latest changes and updating my changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -634,8 +634,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -668,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -696,7 +696,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -710,7 +710,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -724,7 +724,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -738,7 +738,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -752,7 +752,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -766,7 +766,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -780,7 +780,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -794,7 +794,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -808,7 +808,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -822,7 +822,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -850,7 +850,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -864,7 +864,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -878,7 +878,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -892,7 +892,7 @@
         <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Running all the suites
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -634,7 +631,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -667,7 +664,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -695,7 +692,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -709,7 +706,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -723,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -737,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -751,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -765,7 +762,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -779,7 +776,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -793,7 +790,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -807,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -821,7 +818,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -835,7 +832,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -849,7 +846,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -863,7 +860,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -877,7 +874,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -891,7 +888,7 @@
         <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Running a2,a4 and b6
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -251,6 +251,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -634,15 +635,15 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:C18"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -667,7 +668,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -681,7 +682,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>19</v>
@@ -709,10 +710,10 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -912,10 +913,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -959,8 +960,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -974,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1039,8 +1040,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1054,7 +1055,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1119,9 +1120,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1135,7 +1136,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1239,9 +1240,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1255,7 +1256,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1359,9 +1360,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1375,7 +1376,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1479,10 +1480,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1502,7 +1503,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1618,9 +1619,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1634,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1686,11 +1687,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1710,7 +1711,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
running A suite test case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
   <si>
     <t>TCID</t>
   </si>
@@ -242,6 +242,9 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>N</t>
   </si>
 </sst>
 </file>
@@ -631,7 +634,7 @@
   <dimension ref="A1:D18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,10 +667,10 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -678,7 +681,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -692,7 +695,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -706,7 +709,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -720,7 +723,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -734,7 +737,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -748,7 +751,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -762,7 +765,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -776,7 +779,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -790,7 +793,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -804,7 +807,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -818,7 +821,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -846,7 +849,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -860,7 +863,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -874,7 +877,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -888,7 +891,7 @@
         <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
Runn ing all the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -242,9 +242,6 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
-  </si>
-  <si>
-    <t>N</t>
   </si>
 </sst>
 </file>
@@ -633,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -667,7 +664,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -681,7 +678,7 @@
         <v>62</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>12</v>
@@ -695,7 +692,7 @@
         <v>64</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -709,7 +706,7 @@
         <v>63</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -723,7 +720,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -737,7 +734,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -751,7 +748,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>59</v>
@@ -765,7 +762,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -779,7 +776,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -793,7 +790,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -807,7 +804,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -821,7 +818,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -835,7 +832,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -849,7 +846,7 @@
         <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -863,7 +860,7 @@
         <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -877,7 +874,7 @@
         <v>69</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>11</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>

</xml_diff>

<commit_message>
took latest code changes and append my changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1111,7 +1111,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1132,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1146,7 +1146,7 @@
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1160,7 +1160,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1174,7 +1174,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1184,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1196,7 +1196,7 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1208,7 +1208,7 @@
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running all the test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -751,7 +751,7 @@
         <v>11</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -835,7 +835,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1132,7 +1132,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1174,7 +1174,7 @@
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1184,7 +1184,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>59</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1231,7 +1231,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1260,13 +1260,13 @@
         <v>33</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1274,13 +1274,13 @@
         <v>32</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1288,13 +1288,13 @@
         <v>33</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1316,19 +1316,19 @@
         <v>11</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C7" s="6" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>12</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running failed search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -248,6 +248,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -636,10 +637,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -835,7 +836,7 @@
         <v>11</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -909,10 +910,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -956,8 +957,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1036,8 +1037,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1116,9 +1117,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1236,9 +1237,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1356,9 +1357,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1476,10 +1477,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1615,9 +1616,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1683,11 +1684,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Taking latest changes and appending my changess
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
   <si>
     <t>TCID</t>
   </si>
@@ -211,9 +211,6 @@
     <t>To verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
   </si>
   <si>
-    <t>To verify that existing TR user is able to login and logout successfully</t>
-  </si>
-  <si>
     <t>To verify that existing FB user is able to login and logout successfully</t>
   </si>
   <si>
@@ -242,13 +239,15 @@
   </si>
   <si>
     <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -637,10 +636,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -676,7 +675,7 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>62</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>11</v>
@@ -690,7 +689,7 @@
         <v>8</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>11</v>
@@ -704,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>11</v>
@@ -841,10 +840,10 @@
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>11</v>
@@ -855,10 +854,10 @@
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>11</v>
@@ -869,10 +868,10 @@
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>11</v>
@@ -883,10 +882,10 @@
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B18" s="5" t="s">
         <v>71</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>72</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>11</v>
@@ -910,10 +909,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -957,8 +956,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1037,8 +1036,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1117,9 +1116,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1237,9 +1236,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1357,9 +1356,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1477,10 +1476,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1616,9 +1615,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1684,11 +1683,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Adding test cases in IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -16,14 +16,15 @@
     <sheet name="TestCase_A10" sheetId="10" r:id="rId7"/>
     <sheet name="TestCase_A11" sheetId="11" r:id="rId8"/>
     <sheet name="TestCase_A12" sheetId="12" r:id="rId9"/>
-    <sheet name="Test Case Steps" sheetId="4" r:id="rId10"/>
+    <sheet name="TestCase_A19" sheetId="13" r:id="rId10"/>
+    <sheet name="Test Case Steps" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="86">
   <si>
     <t>TCID</t>
   </si>
@@ -242,6 +243,50 @@
   </si>
   <si>
     <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>TestCase_A18</t>
+  </si>
+  <si>
+    <t>Verify that Linkedin CANCEL button is working correctly</t>
+  </si>
+  <si>
+    <t>TestCase_A19</t>
+  </si>
+  <si>
+    <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new TR user registration page:
+1)        *
+2)        (
+3)        )
+4)        &amp;
+5)        !</t>
+  </si>
+  <si>
+    <t>Special character</t>
+  </si>
+  <si>
+    <t>*</t>
+  </si>
+  <si>
+    <t>(</t>
+  </si>
+  <si>
+    <t>)</t>
+  </si>
+  <si>
+    <t>&amp;</t>
+  </si>
+  <si>
+    <t>!</t>
+  </si>
+  <si>
+    <t>TestCase_A20</t>
+  </si>
+  <si>
+    <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
   </si>
 </sst>
 </file>
@@ -317,7 +362,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -333,6 +378,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -628,10 +676,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C18"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -664,7 +712,7 @@
         <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>12</v>
@@ -692,7 +740,7 @@
         <v>63</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>12</v>
@@ -706,7 +754,7 @@
         <v>62</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>12</v>
@@ -720,7 +768,7 @@
         <v>14</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>12</v>
@@ -734,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>12</v>
@@ -748,7 +796,7 @@
         <v>23</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D8" s="2" t="s">
         <v>12</v>
@@ -762,7 +810,7 @@
         <v>31</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D9" s="2" t="s">
         <v>12</v>
@@ -776,7 +824,7 @@
         <v>35</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D10" s="2" t="s">
         <v>12</v>
@@ -790,7 +838,7 @@
         <v>38</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>12</v>
@@ -804,7 +852,7 @@
         <v>46</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>12</v>
@@ -818,7 +866,7 @@
         <v>48</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D13" s="2" t="s">
         <v>12</v>
@@ -832,7 +880,7 @@
         <v>61</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>12</v>
@@ -846,7 +894,7 @@
         <v>65</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D15" s="2" t="s">
         <v>12</v>
@@ -860,7 +908,7 @@
         <v>67</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>12</v>
@@ -874,7 +922,7 @@
         <v>68</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D17" s="2" t="s">
         <v>12</v>
@@ -888,9 +936,51 @@
         <v>71</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>11</v>
+        <v>73</v>
       </c>
       <c r="D18" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="B19" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="C19" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="90">
+      <c r="A20" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D21" s="2" t="s">
         <v>12</v>
       </c>
     </row>
@@ -900,6 +990,96 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="amneetsingh72@gmail.com"/>
+    <hyperlink ref="A4" r:id="rId2" display="amneetsinghasr@gmail.com"/>
+    <hyperlink ref="A3" r:id="rId3" display="amneetsingh100@gmail.com"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -1471,7 +1651,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Suite A excel changed
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -41,18 +41,21 @@
     <t>TestCase_A1</t>
   </si>
   <si>
+    <t>TestCase_A2</t>
+  </si>
+  <si>
     <t>TC SCENARIO</t>
   </si>
   <si>
     <t>TC STEPS</t>
   </si>
   <si>
+    <t>TestCase_A3</t>
+  </si>
+  <si>
     <t>TestCase_A4</t>
   </si>
   <si>
-    <t>To verify that new user is able to register TR new account and login with that</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -62,9 +65,6 @@
     <t>TestCase_A5</t>
   </si>
   <si>
-    <t>To verify FIRST NAME field in new TR user registration page</t>
-  </si>
-  <si>
     <t>VALIDITY</t>
   </si>
   <si>
@@ -83,15 +83,9 @@
     <t>TestCase_A6</t>
   </si>
   <si>
-    <t>To verify LAST NAME field in new TR user registration page</t>
-  </si>
-  <si>
     <t>TestCase_A7</t>
   </si>
   <si>
-    <t>To verify that user is not able to login using FB option for different negative combinations of username/password</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
@@ -113,9 +107,6 @@
     <t>TestCase_A8</t>
   </si>
   <si>
-    <t>To verify that user is not able to login using LI option for different negative combinations of username/password</t>
-  </si>
-  <si>
     <t>amneetsingh100@gmail.com</t>
   </si>
   <si>
@@ -125,18 +116,12 @@
     <t>TestCase_A9</t>
   </si>
   <si>
-    <t>To verify that user is not able to login using TR option for different negative combinations of username/password</t>
-  </si>
-  <si>
     <t>amneet.singh@thomsonreuters.com</t>
   </si>
   <si>
     <t>amneetsingh@thomsonreuters.com</t>
   </si>
   <si>
-    <t>To verify EMAIL ADDRESS field in new TR user registration page</t>
-  </si>
-  <si>
     <t>TestCase_A10</t>
   </si>
   <si>
@@ -158,15 +143,9 @@
     <t>TestCase_A11</t>
   </si>
   <si>
-    <t>To verify CONFIRM PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
     <t>TestCase_A12</t>
   </si>
   <si>
-    <t>To verify PASSWORD field in new TR user registration page</t>
-  </si>
-  <si>
     <t>STRENGTH</t>
   </si>
   <si>
@@ -203,37 +182,16 @@
     <t>TestCase_A13</t>
   </si>
   <si>
-    <t>To verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
-  </si>
-  <si>
-    <t>To verify that existing FB user is able to login and logout successfully</t>
-  </si>
-  <si>
-    <t>To verify that existing LI user is able to login and logout successfully</t>
-  </si>
-  <si>
     <t>TestCase_A14</t>
   </si>
   <si>
-    <t>To verify that user is not able to submit new TR user registration form without filling in the required fields</t>
-  </si>
-  <si>
     <t>TestCase_A15</t>
   </si>
   <si>
-    <t>To verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
-  </si>
-  <si>
-    <t>To verify that user is able to change his TR password by using FORGOT YOUR PASSWORD link and that he is able to login with his new password</t>
-  </si>
-  <si>
     <t>TestCase_A16</t>
   </si>
   <si>
     <t>TestCase_A17</t>
-  </si>
-  <si>
-    <t>To verify that name of a user is truncated using ellipse if the name is very long</t>
   </si>
   <si>
     <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process</t>
@@ -280,35 +238,121 @@
     <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>TestCase_A2</t>
-  </si>
-  <si>
     <t>Jira id</t>
   </si>
   <si>
-    <t>OPQA-10</t>
-  </si>
-  <si>
-    <t>OPQA-10|OPQA-23</t>
-  </si>
-  <si>
-    <t>TestCase_A3</t>
-  </si>
-  <si>
-    <t>OPQA-201</t>
-  </si>
-  <si>
-    <t>OPQA-189</t>
+    <t>Verify that user is able to register for a new TR account and is able to login with that</t>
+  </si>
+  <si>
+    <t>Verify that user is able to login with existing LI id and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify that existing FB user is able to login and logout successfully</t>
+  </si>
+  <si>
+    <t>Verify FIRST NAME field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify LAST NAME field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using FB option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using LI option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to login using TR option for different negative combinations of username/password</t>
+  </si>
+  <si>
+    <t>Verify EMAIL ADDRESS field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify CONFIRM PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify PASSWORD field in new TR user registration page</t>
+  </si>
+  <si>
+    <t>Verify that TERMS OF USE and PRIVACY STATEMENT links are working correctly</t>
+  </si>
+  <si>
+    <t>Verify that user is not able to submit new TR user registration form without filling in the required fields</t>
+  </si>
+  <si>
+    <t>Verify that app doesn't allow the user to create a new account with an email id that has already been used</t>
+  </si>
+  <si>
+    <t>Verify that user is able to change his TR password by using FORGOT YOUR PASSWORD link and that he is able to login with his new password</t>
+  </si>
+  <si>
+    <t>Verify that name of a user is truncated using ellipse if the name is very long</t>
+  </si>
+  <si>
+    <t>OPQA-205</t>
+  </si>
+  <si>
+    <t>OPQA-335</t>
+  </si>
+  <si>
+    <t>OPQA-346</t>
+  </si>
+  <si>
+    <t>OPQA-350</t>
+  </si>
+  <si>
+    <t>OPQA-391</t>
+  </si>
+  <si>
+    <t>OPQA-393</t>
+  </si>
+  <si>
+    <t>OPQA-353</t>
+  </si>
+  <si>
+    <t>OPQA-355</t>
+  </si>
+  <si>
+    <t>OPQA-356</t>
+  </si>
+  <si>
+    <t>OPQA-357</t>
+  </si>
+  <si>
+    <t>OPQA-395</t>
+  </si>
+  <si>
+    <t>OPQA-394</t>
+  </si>
+  <si>
+    <t>OPQA-397</t>
+  </si>
+  <si>
+    <t>OPQA-400</t>
+  </si>
+  <si>
+    <t>OPQA-523</t>
+  </si>
+  <si>
+    <t>OPQA-535</t>
+  </si>
+  <si>
+    <t>OPQA-538</t>
+  </si>
+  <si>
+    <t>OPQA-724</t>
+  </si>
+  <si>
+    <t>OPQA-725</t>
+  </si>
+  <si>
+    <t>OPQA-551</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -333,7 +377,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -343,6 +387,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -378,7 +428,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -395,6 +445,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -694,15 +747,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.28515625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -710,7 +764,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>85</v>
+        <v>69</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -729,45 +783,45 @@
       <c r="B2" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>8</v>
+      <c r="C2" s="10" t="s">
+        <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>84</v>
+        <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
+      </c>
+      <c r="C3" s="10" t="s">
+        <v>56</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>61</v>
+      <c r="C4" s="10" t="s">
+        <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>17</v>
@@ -775,291 +829,291 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>60</v>
+        <v>89</v>
+      </c>
+      <c r="C5" s="10" t="s">
+        <v>72</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" s="6" t="s">
         <v>12</v>
       </c>
+      <c r="B6" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>73</v>
+      </c>
       <c r="D6" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>19</v>
+      <c r="B7" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>76</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>33</v>
+        <v>29</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>77</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>36</v>
+        <v>32</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="5" t="s">
+        <v>78</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="6" t="s">
-        <v>44</v>
+        <v>38</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C13" s="6" t="s">
-        <v>46</v>
+        <v>39</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>86</v>
+        <v>51</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>98</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>59</v>
+        <v>81</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>63</v>
+        <v>52</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>82</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>65</v>
+        <v>53</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>66</v>
+        <v>54</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>84</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>86</v>
+        <v>55</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>69</v>
+        <v>85</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="2" t="s">
-        <v>86</v>
+        <v>57</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>103</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>10</v>
+        <v>50</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90">
       <c r="A20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>90</v>
+        <v>59</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>104</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>74</v>
+        <v>60</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>89</v>
+        <v>67</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>105</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>82</v>
+        <v>68</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>83</v>
+        <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1077,13 +1131,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>75</v>
+        <v>61</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
@@ -1094,10 +1148,10 @@
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>17</v>
@@ -1105,10 +1159,10 @@
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>17</v>
@@ -1116,10 +1170,10 @@
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>78</v>
+        <v>64</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
@@ -1127,10 +1181,10 @@
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>17</v>
@@ -1138,10 +1192,10 @@
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
@@ -1167,10 +1221,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1178,10 +1232,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1">
@@ -1214,8 +1268,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1240,10 +1294,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1254,10 +1308,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1268,7 +1322,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
@@ -1294,8 +1348,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1320,10 +1374,10 @@
         <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1334,10 +1388,10 @@
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1348,7 +1402,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
@@ -1374,17 +1428,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1395,13 +1449,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1409,13 +1463,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1423,13 +1477,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
@@ -1439,7 +1493,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -1447,11 +1501,11 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
@@ -1460,10 +1514,10 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -1494,17 +1548,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1515,13 +1569,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1529,13 +1583,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1543,13 +1597,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
@@ -1559,7 +1613,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -1567,11 +1621,11 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
@@ -1580,10 +1634,10 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -1614,17 +1668,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
@@ -1635,13 +1689,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1649,13 +1703,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1663,13 +1717,13 @@
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>17</v>
@@ -1679,7 +1733,7 @@
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>17</v>
@@ -1687,11 +1741,11 @@
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D6" s="2" t="s">
         <v>17</v>
@@ -1700,10 +1754,10 @@
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>17</v>
@@ -1734,10 +1788,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1745,10 +1799,10 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1765,17 +1819,17 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1783,17 +1837,17 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1801,19 +1855,19 @@
         <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="D4" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1822,13 +1876,13 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>17</v>
@@ -1839,14 +1893,14 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>17</v>
@@ -1873,14 +1927,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>13</v>
@@ -1894,13 +1948,13 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>15</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>17</v>
@@ -1908,13 +1962,13 @@
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>17</v>
@@ -1941,22 +1995,22 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>13</v>
@@ -1970,10 +2024,10 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
@@ -1982,18 +2036,18 @@
         <v>15</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
@@ -2002,18 +2056,18 @@
         <v>15</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
@@ -2022,18 +2076,18 @@
         <v>15</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
@@ -2042,18 +2096,18 @@
         <v>15</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
@@ -2062,10 +2116,10 @@
         <v>14</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changes in b suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="394" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -353,6 +353,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -753,10 +754,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -790,7 +791,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -807,7 +808,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -824,7 +825,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -841,7 +842,7 @@
         <v>10</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -858,7 +859,7 @@
         <v>10</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -875,7 +876,7 @@
         <v>10</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5">
@@ -892,7 +893,7 @@
         <v>10</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -909,7 +910,7 @@
         <v>10</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -926,7 +927,7 @@
         <v>10</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:5">
@@ -943,7 +944,7 @@
         <v>10</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -960,7 +961,7 @@
         <v>10</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -977,7 +978,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -994,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1011,7 +1012,7 @@
         <v>10</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="16" spans="1:5">
@@ -1028,7 +1029,7 @@
         <v>10</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -1045,7 +1046,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1062,7 +1063,7 @@
         <v>10</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -1079,7 +1080,7 @@
         <v>10</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>50</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90">
@@ -1096,7 +1097,7 @@
         <v>10</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1113,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1131,8 +1132,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1221,10 +1222,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1268,8 +1269,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1348,8 +1349,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1428,9 +1429,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1548,9 +1549,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1668,9 +1669,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1788,10 +1789,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1927,9 +1928,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1995,11 +1996,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Fix for IAM related test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="106">
   <si>
     <t>TCID</t>
   </si>
@@ -353,6 +353,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -747,16 +748,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -994,7 +995,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1131,8 +1132,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1221,10 +1222,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1268,8 +1269,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1348,8 +1349,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1428,9 +1429,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1548,9 +1549,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1668,9 +1669,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1788,10 +1789,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1927,9 +1928,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1995,11 +1996,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
taking latest changes and appending new changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="116">
   <si>
     <t>TCID</t>
   </si>
@@ -348,12 +348,41 @@
   <si>
     <t>OPQA-551</t>
   </si>
+  <si>
+    <t>TestCase_A21</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>TestCase_A22</t>
+  </si>
+  <si>
+    <t>TestCase_A23</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -746,18 +775,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -788,7 +818,7 @@
         <v>70</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>11</v>
@@ -805,7 +835,7 @@
         <v>56</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>11</v>
@@ -822,7 +852,7 @@
         <v>71</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>11</v>
@@ -839,7 +869,7 @@
         <v>72</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>11</v>
@@ -856,7 +886,7 @@
         <v>73</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>11</v>
@@ -873,7 +903,7 @@
         <v>74</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>11</v>
@@ -890,7 +920,7 @@
         <v>75</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>11</v>
@@ -907,7 +937,7 @@
         <v>76</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>11</v>
@@ -924,7 +954,7 @@
         <v>77</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>11</v>
@@ -941,7 +971,7 @@
         <v>78</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>11</v>
@@ -958,7 +988,7 @@
         <v>79</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>11</v>
@@ -975,7 +1005,7 @@
         <v>80</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>11</v>
@@ -992,7 +1022,7 @@
         <v>81</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>11</v>
@@ -1009,7 +1039,7 @@
         <v>82</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>11</v>
@@ -1026,7 +1056,7 @@
         <v>83</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>11</v>
@@ -1043,7 +1073,7 @@
         <v>84</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>11</v>
@@ -1060,7 +1090,7 @@
         <v>85</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>11</v>
@@ -1077,7 +1107,7 @@
         <v>58</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>11</v>
@@ -1094,7 +1124,7 @@
         <v>60</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>11</v>
@@ -1111,14 +1141,66 @@
         <v>68</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="E21" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E24" s="2" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1132,8 +1214,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1222,10 +1304,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1269,8 +1351,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1349,8 +1431,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,9 +1511,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1549,9 +1631,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1669,9 +1751,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1789,10 +1871,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1928,9 +2010,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1996,11 +2078,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
running whole A suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -348,12 +348,38 @@
   <si>
     <t>OPQA-551</t>
   </si>
+  <si>
+    <t>TestCase_A21</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>TestCase_A22</t>
+  </si>
+  <si>
+    <t>TestCase_A23</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -746,18 +772,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1117,8 +1144,60 @@
         <v>11</v>
       </c>
     </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1132,8 +1211,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1222,10 +1301,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1269,8 +1348,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1349,8 +1428,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,9 +1508,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1549,9 +1628,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1669,9 +1748,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1789,10 +1868,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1928,9 +2007,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1996,11 +2075,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Search test cases modified
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -348,12 +348,38 @@
   <si>
     <t>OPQA-551</t>
   </si>
+  <si>
+    <t>TestCase_A21</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>TestCase_A22</t>
+  </si>
+  <si>
+    <t>TestCase_A23</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -746,18 +772,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1117,8 +1144,60 @@
         <v>11</v>
       </c>
     </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1132,8 +1211,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1222,10 +1301,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1269,8 +1348,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1349,8 +1428,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,9 +1508,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1549,9 +1628,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1669,9 +1748,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1789,10 +1868,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1928,9 +2007,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1996,11 +2075,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
adding my changes to remote
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D24"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1073,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">

</xml_diff>

<commit_message>
Taking the latest code
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -348,12 +348,38 @@
   <si>
     <t>OPQA-551</t>
   </si>
+  <si>
+    <t>TestCase_A21</t>
+  </si>
+  <si>
+    <t>Verify View additional email preferences link is working</t>
+  </si>
+  <si>
+    <t>TestCase_A22</t>
+  </si>
+  <si>
+    <t>TestCase_A23</t>
+  </si>
+  <si>
+    <t>Verify change password link in the account page is working correctly.</t>
+  </si>
+  <si>
+    <t>Verify that the  checkbox  is present and can be modified for "Receive email notifications for likes,comments and other activity" is working correctly.</t>
+  </si>
+  <si>
+    <t>OPQA-854,OPQA-853</t>
+  </si>
+  <si>
+    <t>OPQA-399</t>
+  </si>
+  <si>
+    <t>OPQA-527</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -746,18 +772,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="2" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1046,7 +1073,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1117,8 +1144,60 @@
         <v>11</v>
       </c>
     </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="30">
+      <c r="A23" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C23" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1132,8 +1211,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1222,10 +1301,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1269,8 +1348,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1349,8 +1428,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,9 +1508,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1549,9 +1628,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1669,9 +1748,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1789,10 +1868,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1928,9 +2007,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1996,11 +2075,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Commiting changes to local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -774,8 +774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1022,7 +1022,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:5">

</xml_diff>

<commit_message>
Taking latest changes and appending my changes
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="115">
   <si>
     <t>TCID</t>
   </si>
@@ -380,6 +380,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -780,11 +781,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1022,7 +1023,7 @@
         <v>10</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1073,7 +1074,7 @@
         <v>10</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:5">
@@ -1211,8 +1212,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1301,10 +1302,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1348,8 +1349,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1428,8 +1429,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1508,9 +1509,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1628,9 +1629,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1748,9 +1749,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1868,10 +1869,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2007,9 +2008,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2075,11 +2076,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Adding TestCases for IAM
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
   <si>
     <t>TCID</t>
   </si>
@@ -375,12 +375,29 @@
   <si>
     <t>OPQA-527</t>
   </si>
+  <si>
+    <t>TestCase_A24</t>
+  </si>
+  <si>
+    <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
+  </si>
+  <si>
+    <t>OPQA-525</t>
+  </si>
+  <si>
+    <t>TestCase_A25</t>
+  </si>
+  <si>
+    <t>OPQA-529</t>
+  </si>
+  <si>
+    <t>Verify that Help link is working properly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -773,19 +790,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1194,6 +1211,40 @@
       </c>
       <c r="E24" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1212,8 +1263,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1302,10 +1353,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1349,8 +1400,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,8 +1480,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1509,9 +1560,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1629,9 +1680,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1749,9 +1800,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1869,10 +1920,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2008,9 +2059,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2076,11 +2127,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Fixing scripts for watch list
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
   <si>
     <t>TCID</t>
   </si>
@@ -375,12 +375,29 @@
   <si>
     <t>OPQA-527</t>
   </si>
+  <si>
+    <t>TestCase_A24</t>
+  </si>
+  <si>
+    <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
+  </si>
+  <si>
+    <t>OPQA-525</t>
+  </si>
+  <si>
+    <t>TestCase_A25</t>
+  </si>
+  <si>
+    <t>OPQA-529</t>
+  </si>
+  <si>
+    <t>Verify that Help link is working properly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -773,19 +790,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1194,6 +1211,40 @@
       </c>
       <c r="E24" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1212,8 +1263,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1302,10 +1353,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1349,8 +1400,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,8 +1480,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1509,9 +1560,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1629,9 +1680,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1749,9 +1800,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1869,10 +1920,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2008,9 +2059,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2076,11 +2127,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Adding 5 search test cases(B68-B72)
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="953" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
   <si>
     <t>TCID</t>
   </si>
@@ -375,12 +375,29 @@
   <si>
     <t>OPQA-527</t>
   </si>
+  <si>
+    <t>TestCase_A24</t>
+  </si>
+  <si>
+    <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
+  </si>
+  <si>
+    <t>OPQA-525</t>
+  </si>
+  <si>
+    <t>TestCase_A25</t>
+  </si>
+  <si>
+    <t>OPQA-529</t>
+  </si>
+  <si>
+    <t>Verify that Help link is working properly</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -773,19 +790,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
+    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -1194,6 +1211,40 @@
       </c>
       <c r="E24" s="2" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1212,8 +1263,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1302,10 +1353,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
-    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
+    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
+    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1349,8 +1400,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1429,8 +1480,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1509,9 +1560,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1629,9 +1680,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1749,9 +1800,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1869,10 +1920,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2008,9 +2059,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2076,11 +2127,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Adding 2 search test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -792,8 +792,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Running only A suite
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -793,7 +793,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1275,7 +1275,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -1415,7 +1415,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1495,7 +1495,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1576,7 +1576,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1696,7 +1696,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1816,7 +1816,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1915,7 +1915,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1943,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -2075,7 +2075,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -2151,7 +2151,7 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:6">

</xml_diff>

<commit_message>
Taking latest changes to local
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -793,7 +793,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,7 +1475,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1915,7 +1915,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
removing thread sleeps from profile testcases
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -793,7 +793,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1244,7 +1244,7 @@
         <v>10</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -1258,7 +1258,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1475,7 +1475,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1555,7 +1555,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1675,7 +1675,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1915,7 +1915,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Fix for IAM test case
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="121">
   <si>
     <t>TCID</t>
   </si>
@@ -398,6 +398,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -798,11 +799,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="130" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="25.28515625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="130.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="7.2578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -836,7 +837,7 @@
         <v>10</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:5">
@@ -853,7 +854,7 @@
         <v>10</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:5">
@@ -870,7 +871,7 @@
         <v>10</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1263,8 +1264,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1353,10 +1354,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="12.140625" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="45.42578125" style="3" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="83.5703125" style="3" customWidth="1" collapsed="1"/>
-    <col min="4" max="16384" width="9.140625" style="3" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="3" width="12.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="3" width="45.42578125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="3" width="83.5703125" collapsed="true"/>
+    <col min="4" max="16384" style="3" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
@@ -1400,8 +1401,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1480,8 +1481,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1560,9 +1561,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1680,9 +1681,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1800,9 +1801,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="34.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="34.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1920,10 +1921,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="19" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="37.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -2059,9 +2060,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="27.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="27.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -2127,11 +2128,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">

</xml_diff>

<commit_message>
Committing changes made in IAM module
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCase_A5" sheetId="5" r:id="rId2"/>
-    <sheet name="TestCase_A6" sheetId="6" r:id="rId3"/>
-    <sheet name="TestCase_A7" sheetId="7" r:id="rId4"/>
-    <sheet name="TestCase_A8" sheetId="8" r:id="rId5"/>
-    <sheet name="TestCase_A9" sheetId="9" r:id="rId6"/>
-    <sheet name="TestCase_A10" sheetId="10" r:id="rId7"/>
-    <sheet name="TestCase_A11" sheetId="11" r:id="rId8"/>
-    <sheet name="TestCase_A12" sheetId="12" r:id="rId9"/>
-    <sheet name="TestCase_A19" sheetId="13" r:id="rId10"/>
+    <sheet name="IAM005" sheetId="5" r:id="rId2"/>
+    <sheet name="IAM006" sheetId="6" r:id="rId3"/>
+    <sheet name="IAM007" sheetId="7" r:id="rId4"/>
+    <sheet name="IAM008" sheetId="8" r:id="rId5"/>
+    <sheet name="IAM009" sheetId="9" r:id="rId6"/>
+    <sheet name="IAM010" sheetId="10" r:id="rId7"/>
+    <sheet name="IAM011" sheetId="11" r:id="rId8"/>
+    <sheet name="IAM012" sheetId="12" r:id="rId9"/>
+    <sheet name="IAM019" sheetId="13" r:id="rId10"/>
     <sheet name="Test Case Steps" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="120">
   <si>
     <t>TCID</t>
   </si>
@@ -35,36 +35,18 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>TestCase_A1</t>
-  </si>
-  <si>
-    <t>TestCase_A2</t>
-  </si>
-  <si>
     <t>TC SCENARIO</t>
   </si>
   <si>
     <t>TC STEPS</t>
   </si>
   <si>
-    <t>TestCase_A3</t>
-  </si>
-  <si>
-    <t>TestCase_A4</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>TestCase_A5</t>
-  </si>
-  <si>
     <t>VALIDITY</t>
   </si>
   <si>
@@ -80,12 +62,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>TestCase_A6</t>
-  </si>
-  <si>
-    <t>TestCase_A7</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
@@ -104,27 +80,18 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>TestCase_A8</t>
-  </si>
-  <si>
     <t>amneetsingh100@gmail.com</t>
   </si>
   <si>
     <t>amneetsingh10@gmail.com</t>
   </si>
   <si>
-    <t>TestCase_A9</t>
-  </si>
-  <si>
     <t>amneet.singh@thomsonreuters.com</t>
   </si>
   <si>
     <t>amneetsingh@thomsonreuters.com</t>
   </si>
   <si>
-    <t>TestCase_A10</t>
-  </si>
-  <si>
     <t>SUFFIX</t>
   </si>
   <si>
@@ -140,12 +107,6 @@
     <t>Please enter a valid Email Address.</t>
   </si>
   <si>
-    <t>TestCase_A11</t>
-  </si>
-  <si>
-    <t>TestCase_A12</t>
-  </si>
-  <si>
     <t>STRENGTH</t>
   </si>
   <si>
@@ -179,31 +140,10 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>TestCase_A13</t>
-  </si>
-  <si>
-    <t>TestCase_A14</t>
-  </si>
-  <si>
-    <t>TestCase_A15</t>
-  </si>
-  <si>
-    <t>TestCase_A16</t>
-  </si>
-  <si>
-    <t>TestCase_A17</t>
-  </si>
-  <si>
     <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process</t>
   </si>
   <si>
-    <t>TestCase_A18</t>
-  </si>
-  <si>
     <t>Verify that Linkedin CANCEL button is working correctly</t>
-  </si>
-  <si>
-    <t>TestCase_A19</t>
   </si>
   <si>
     <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new TR user registration page:
@@ -232,9 +172,6 @@
     <t>!</t>
   </si>
   <si>
-    <t>TestCase_A20</t>
-  </si>
-  <si>
     <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
   </si>
   <si>
@@ -349,18 +286,9 @@
     <t>OPQA-551</t>
   </si>
   <si>
-    <t>TestCase_A21</t>
-  </si>
-  <si>
     <t>Verify View additional email preferences link is working</t>
   </si>
   <si>
-    <t>TestCase_A22</t>
-  </si>
-  <si>
-    <t>TestCase_A23</t>
-  </si>
-  <si>
     <t>Verify change password link in the account page is working correctly.</t>
   </si>
   <si>
@@ -376,22 +304,91 @@
     <t>OPQA-527</t>
   </si>
   <si>
-    <t>TestCase_A24</t>
-  </si>
-  <si>
     <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
   </si>
   <si>
     <t>OPQA-525</t>
   </si>
   <si>
-    <t>TestCase_A25</t>
-  </si>
-  <si>
     <t>OPQA-529</t>
   </si>
   <si>
     <t>Verify that Help link is working properly</t>
+  </si>
+  <si>
+    <t>IAM001</t>
+  </si>
+  <si>
+    <t>IAM002</t>
+  </si>
+  <si>
+    <t>IAM003</t>
+  </si>
+  <si>
+    <t>IAM004</t>
+  </si>
+  <si>
+    <t>IAM005</t>
+  </si>
+  <si>
+    <t>IAM006</t>
+  </si>
+  <si>
+    <t>IAM007</t>
+  </si>
+  <si>
+    <t>IAM008</t>
+  </si>
+  <si>
+    <t>IAM009</t>
+  </si>
+  <si>
+    <t>IAM010</t>
+  </si>
+  <si>
+    <t>IAM011</t>
+  </si>
+  <si>
+    <t>IAM012</t>
+  </si>
+  <si>
+    <t>IAM019</t>
+  </si>
+  <si>
+    <t>IAM013</t>
+  </si>
+  <si>
+    <t>IAM014</t>
+  </si>
+  <si>
+    <t>IAM015</t>
+  </si>
+  <si>
+    <t>IAM016</t>
+  </si>
+  <si>
+    <t>IAM017</t>
+  </si>
+  <si>
+    <t>IAM018</t>
+  </si>
+  <si>
+    <t>IAM020</t>
+  </si>
+  <si>
+    <t>IAM021</t>
+  </si>
+  <si>
+    <t>IAM022</t>
+  </si>
+  <si>
+    <t>IAM023</t>
+  </si>
+  <si>
+    <t>IAM024</t>
+  </si>
+  <si>
+    <t>IAM025</t>
   </si>
 </sst>
 </file>
@@ -803,7 +800,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -820,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -829,432 +826,432 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90">
       <c r="A20" s="6" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>106</v>
+      <c r="A22" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1279,68 +1276,68 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1374,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1">
@@ -1405,7 +1402,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,16 +1413,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1433,13 +1430,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1447,13 +1444,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1461,13 +1458,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1478,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1492,16 +1489,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1509,13 +1506,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1523,13 +1520,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1537,13 +1534,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1568,92 +1565,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1688,92 +1685,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1808,92 +1805,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1929,22 +1926,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1952,17 +1949,17 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1970,17 +1967,17 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1988,19 +1985,19 @@
         <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2009,16 +2006,16 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2026,17 +2023,17 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2067,44 +2064,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2137,122 +2134,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Committing after Formatting all modules
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -799,8 +799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2120,7 +2120,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Taking the updated code
</commit_message>
<xml_diff>
--- a/src/test/resources/xls/A suite.xlsx
+++ b/src/test/resources/xls/A suite.xlsx
@@ -8,15 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
-    <sheet name="TestCase_A5" sheetId="5" r:id="rId2"/>
-    <sheet name="TestCase_A6" sheetId="6" r:id="rId3"/>
-    <sheet name="TestCase_A7" sheetId="7" r:id="rId4"/>
-    <sheet name="TestCase_A8" sheetId="8" r:id="rId5"/>
-    <sheet name="TestCase_A9" sheetId="9" r:id="rId6"/>
-    <sheet name="TestCase_A10" sheetId="10" r:id="rId7"/>
-    <sheet name="TestCase_A11" sheetId="11" r:id="rId8"/>
-    <sheet name="TestCase_A12" sheetId="12" r:id="rId9"/>
-    <sheet name="TestCase_A19" sheetId="13" r:id="rId10"/>
+    <sheet name="IAM005" sheetId="5" r:id="rId2"/>
+    <sheet name="IAM006" sheetId="6" r:id="rId3"/>
+    <sheet name="IAM007" sheetId="7" r:id="rId4"/>
+    <sheet name="IAM008" sheetId="8" r:id="rId5"/>
+    <sheet name="IAM009" sheetId="9" r:id="rId6"/>
+    <sheet name="IAM010" sheetId="10" r:id="rId7"/>
+    <sheet name="IAM011" sheetId="11" r:id="rId8"/>
+    <sheet name="IAM012" sheetId="12" r:id="rId9"/>
+    <sheet name="IAM019" sheetId="13" r:id="rId10"/>
     <sheet name="Test Case Steps" sheetId="4" r:id="rId11"/>
   </sheets>
   <calcPr calcId="125725"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="120">
   <si>
     <t>TCID</t>
   </si>
@@ -35,36 +35,18 @@
     <t>Runmode</t>
   </si>
   <si>
-    <t>Results</t>
-  </si>
-  <si>
-    <t>TestCase_A1</t>
-  </si>
-  <si>
-    <t>TestCase_A2</t>
-  </si>
-  <si>
     <t>TC SCENARIO</t>
   </si>
   <si>
     <t>TC STEPS</t>
   </si>
   <si>
-    <t>TestCase_A3</t>
-  </si>
-  <si>
-    <t>TestCase_A4</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
     <t>SKIP</t>
   </si>
   <si>
-    <t>TestCase_A5</t>
-  </si>
-  <si>
     <t>VALIDITY</t>
   </si>
   <si>
@@ -80,12 +62,6 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>TestCase_A6</t>
-  </si>
-  <si>
-    <t>TestCase_A7</t>
-  </si>
-  <si>
     <t>PASSWORD</t>
   </si>
   <si>
@@ -104,27 +80,18 @@
     <t>EMAIL</t>
   </si>
   <si>
-    <t>TestCase_A8</t>
-  </si>
-  <si>
     <t>amneetsingh100@gmail.com</t>
   </si>
   <si>
     <t>amneetsingh10@gmail.com</t>
   </si>
   <si>
-    <t>TestCase_A9</t>
-  </si>
-  <si>
     <t>amneet.singh@thomsonreuters.com</t>
   </si>
   <si>
     <t>amneetsingh@thomsonreuters.com</t>
   </si>
   <si>
-    <t>TestCase_A10</t>
-  </si>
-  <si>
     <t>SUFFIX</t>
   </si>
   <si>
@@ -140,12 +107,6 @@
     <t>Please enter a valid Email Address.</t>
   </si>
   <si>
-    <t>TestCase_A11</t>
-  </si>
-  <si>
-    <t>TestCase_A12</t>
-  </si>
-  <si>
     <t>STRENGTH</t>
   </si>
   <si>
@@ -179,31 +140,10 @@
     <t>FAIL</t>
   </si>
   <si>
-    <t>TestCase_A13</t>
-  </si>
-  <si>
-    <t>TestCase_A14</t>
-  </si>
-  <si>
-    <t>TestCase_A15</t>
-  </si>
-  <si>
-    <t>TestCase_A16</t>
-  </si>
-  <si>
-    <t>TestCase_A17</t>
-  </si>
-  <si>
     <t>Verify that existing TR user is able to login successfully and that case-sensitivity of email id doesn't have any effect on login process</t>
   </si>
   <si>
-    <t>TestCase_A18</t>
-  </si>
-  <si>
     <t>Verify that Linkedin CANCEL button is working correctly</t>
-  </si>
-  <si>
-    <t>TestCase_A19</t>
   </si>
   <si>
     <t>Verify that following special characters are not allowed in EMAIL ADDRESS field in new TR user registration page:
@@ -232,9 +172,6 @@
     <t>!</t>
   </si>
   <si>
-    <t>TestCase_A20</t>
-  </si>
-  <si>
     <t>Verify that CREATE A NEW PROJECT NEON ACCOUNT button is working correctly</t>
   </si>
   <si>
@@ -349,18 +286,9 @@
     <t>OPQA-551</t>
   </si>
   <si>
-    <t>TestCase_A21</t>
-  </si>
-  <si>
     <t>Verify View additional email preferences link is working</t>
   </si>
   <si>
-    <t>TestCase_A22</t>
-  </si>
-  <si>
-    <t>TestCase_A23</t>
-  </si>
-  <si>
     <t>Verify change password link in the account page is working correctly.</t>
   </si>
   <si>
@@ -376,22 +304,91 @@
     <t>OPQA-527</t>
   </si>
   <si>
-    <t>TestCase_A24</t>
-  </si>
-  <si>
     <t>Verify that TR account gets locked after 5 consecutive unsuccessful login attempts</t>
   </si>
   <si>
     <t>OPQA-525</t>
   </si>
   <si>
-    <t>TestCase_A25</t>
-  </si>
-  <si>
     <t>OPQA-529</t>
   </si>
   <si>
     <t>Verify that Help link is working properly</t>
+  </si>
+  <si>
+    <t>IAM001</t>
+  </si>
+  <si>
+    <t>IAM002</t>
+  </si>
+  <si>
+    <t>IAM003</t>
+  </si>
+  <si>
+    <t>IAM004</t>
+  </si>
+  <si>
+    <t>IAM005</t>
+  </si>
+  <si>
+    <t>IAM006</t>
+  </si>
+  <si>
+    <t>IAM007</t>
+  </si>
+  <si>
+    <t>IAM008</t>
+  </si>
+  <si>
+    <t>IAM009</t>
+  </si>
+  <si>
+    <t>IAM010</t>
+  </si>
+  <si>
+    <t>IAM011</t>
+  </si>
+  <si>
+    <t>IAM012</t>
+  </si>
+  <si>
+    <t>IAM019</t>
+  </si>
+  <si>
+    <t>IAM013</t>
+  </si>
+  <si>
+    <t>IAM014</t>
+  </si>
+  <si>
+    <t>IAM015</t>
+  </si>
+  <si>
+    <t>IAM016</t>
+  </si>
+  <si>
+    <t>IAM017</t>
+  </si>
+  <si>
+    <t>IAM018</t>
+  </si>
+  <si>
+    <t>IAM020</t>
+  </si>
+  <si>
+    <t>IAM021</t>
+  </si>
+  <si>
+    <t>IAM022</t>
+  </si>
+  <si>
+    <t>IAM023</t>
+  </si>
+  <si>
+    <t>IAM024</t>
+  </si>
+  <si>
+    <t>IAM025</t>
   </si>
 </sst>
 </file>
@@ -820,7 +817,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -829,432 +826,432 @@
         <v>2</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>3</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>95</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>96</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>8</v>
+        <v>97</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>9</v>
+        <v>98</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="6" t="s">
-        <v>12</v>
+        <v>99</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="6" t="s">
-        <v>18</v>
+        <v>100</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="6" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="6" t="s">
-        <v>26</v>
+        <v>102</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="6" t="s">
-        <v>29</v>
+        <v>103</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="6" t="s">
-        <v>32</v>
+        <v>104</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="6" t="s">
-        <v>38</v>
+        <v>105</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="6" t="s">
-        <v>39</v>
+        <v>106</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="6" t="s">
-        <v>51</v>
+        <v>108</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="6" t="s">
-        <v>52</v>
+        <v>109</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="6" t="s">
-        <v>53</v>
+        <v>110</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="C16" s="5" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="6" t="s">
-        <v>54</v>
+        <v>111</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="6" t="s">
-        <v>55</v>
+        <v>112</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="6" t="s">
-        <v>57</v>
+        <v>113</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>58</v>
+        <v>39</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="90">
       <c r="A20" s="6" t="s">
-        <v>59</v>
+        <v>107</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="C20" s="5" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="6" t="s">
-        <v>67</v>
+        <v>114</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:5">
-      <c r="A22" s="2" t="s">
-        <v>106</v>
+      <c r="A22" s="6" t="s">
+        <v>115</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>113</v>
+        <v>89</v>
       </c>
       <c r="C22" s="9" t="s">
-        <v>107</v>
+        <v>85</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30">
       <c r="A23" s="6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>112</v>
+        <v>88</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="D23" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="6" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>114</v>
+        <v>90</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="6" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>117</v>
+        <v>92</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>116</v>
+        <v>91</v>
       </c>
       <c r="D25" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="6" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>119</v>
+        <v>93</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>120</v>
+        <v>94</v>
       </c>
       <c r="D26" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1279,68 +1276,68 @@
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" s="1" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="7" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="7" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:3">
       <c r="A4" s="7" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:3">
       <c r="A5" s="2" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3">
       <c r="A6" s="2" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1374,10 +1371,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="48" customHeight="1">
@@ -1405,7 +1402,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1416,16 +1413,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1433,13 +1430,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1447,13 +1444,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1461,13 +1458,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1481,7 +1478,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="D33" sqref="D33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1492,16 +1489,16 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1509,13 +1506,13 @@
         <v>69</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1523,13 +1520,13 @@
         <v>70</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1537,13 +1534,13 @@
         <v>71</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1568,92 +1565,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1688,92 +1685,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1808,92 +1805,92 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="7" t="s">
-        <v>31</v>
+        <v>21</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2"/>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="7" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2"/>
       <c r="B7" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -1929,22 +1926,22 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>33</v>
+        <v>22</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1952,17 +1949,17 @@
         <v>61</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C2" s="7"/>
       <c r="D2" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1970,17 +1967,17 @@
         <v>62</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
@@ -1988,19 +1985,19 @@
         <v>63</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C4" s="7" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -2009,16 +2006,16 @@
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:6">
@@ -2026,17 +2023,17 @@
         <v>11</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="C6" s="7"/>
       <c r="D6" s="8" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2067,44 +2064,44 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -2123,7 +2120,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2137,122 +2134,122 @@
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C2" s="2">
         <v>1</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="2" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="C3" s="2">
         <v>2</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C4" s="2">
         <v>3</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="C5" s="2">
         <v>4</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="2" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="C6" s="2">
         <v>5</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>